<commit_message>
update the direction of gull wing leds
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="644">
   <si>
     <t>C52,C53,C54,C55,C64,C76,C77,C78,C81,C86,C87,C88,C89,C90,C91,C92,C93,C94,C95,C96,C97,C98,C99,C104,C105,C106,C107,C108,C109,C110,C111,C112,C113,C114,C115,C116,C117,C118,C119,C120,C126,C127,C128,C129,C130,C131,C132,C133,C134,C135,C136,C137,C138,C139,C140,C141,C142,C143,C145,C146,C147,C148,C149,C150,C151,C152,C153,C154,C155,C156,C157,C158,C159,C160,C161,C162,C163,C164,C165,C166,C167,C169,C170,C172,C173,C174,C175,C176,C177,C187,C233,C236,C239,C241,C284,C285</t>
   </si>
@@ -355,9 +355,6 @@
     <t>sot323avx</t>
   </si>
   <si>
-    <t>NXP Semiconductors</t>
-  </si>
-  <si>
     <t>D5,D9</t>
   </si>
   <si>
@@ -1834,9 +1831,6 @@
     <t>LNJ107W5PRW</t>
   </si>
   <si>
-    <t>1.72V RED, 2.03V GRN</t>
-  </si>
-  <si>
     <t>4-SMD_Gull_Wing</t>
   </si>
   <si>
@@ -1852,9 +1846,6 @@
     <t>EEE-FK1E101XP</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/LNJ107W5PRW/P526CT-ND/231474</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/0532610471/WM7622CT-ND/699109</t>
   </si>
   <si>
@@ -1904,9 +1895,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/FDN340P/FDN340PCT-ND/965604</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/BAT54SW,115/568-1615-1-ND/763442</t>
   </si>
   <si>
     <t>http://www.coilcraft.com/pn/XFL4020-222MEB.htm</t>
@@ -1944,6 +1932,24 @@
   <si>
     <t xml:space="preserve">  
 Bourns</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/Search/ProductDetail.aspx?qs=vLkC5FC1VN%252b2vnDL%2fWJ0Ww%3d%3d</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>BAT54SWT1G</t>
+  </si>
+  <si>
+    <t>LN2162C68TR</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LN2162C68TR/P11147CT-ND/341201</t>
+  </si>
+  <si>
+    <t>1.95V ORG, 2.05V GRN</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1960,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;?????_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2118,6 +2124,12 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2523,12 +2535,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2876,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,43 +2910,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>447</v>
-      </c>
       <c r="L1" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>600</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2969,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L2" s="10">
         <v>8.9999999999999993E-3</v>
@@ -3008,10 +3020,10 @@
         <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="L3" s="11">
         <v>1.4E-2</v>
@@ -3050,10 +3062,10 @@
         <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="L4" s="12">
         <v>0.95</v>
@@ -3092,10 +3104,10 @@
         <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L5" s="12">
         <v>0.81</v>
@@ -3137,7 +3149,7 @@
         <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="L6" s="12">
         <v>0.255</v>
@@ -3176,10 +3188,10 @@
         <v>22</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="L7" s="12">
         <v>1.7000000000000001E-2</v>
@@ -3221,7 +3233,7 @@
         <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L8" s="12">
         <v>5.5E-2</v>
@@ -3263,7 +3275,7 @@
         <v>31</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L9" s="12">
         <v>1.2999999999999999E-2</v>
@@ -3305,7 +3317,7 @@
         <v>33</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L10" s="12">
         <v>0.128</v>
@@ -3344,10 +3356,10 @@
         <v>22</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="L11" s="12">
         <v>0.21199999999999999</v>
@@ -3389,7 +3401,7 @@
         <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L12" s="12">
         <v>0.1</v>
@@ -3431,7 +3443,7 @@
         <v>44</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L13" s="12">
         <v>0.74099999999999999</v>
@@ -3473,7 +3485,7 @@
         <v>47</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L14" s="12">
         <v>1.7999999999999999E-2</v>
@@ -3512,10 +3524,10 @@
         <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="L15" s="12">
         <v>7.0000000000000001E-3</v>
@@ -3557,7 +3569,7 @@
         <v>52</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L16" s="12">
         <v>0.185</v>
@@ -3599,7 +3611,7 @@
         <v>56</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L17" s="12">
         <v>1.2999999999999999E-2</v>
@@ -3638,10 +3650,10 @@
         <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="L18" s="12">
         <v>1.08</v>
@@ -3677,10 +3689,10 @@
         <v>11</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L19" s="12">
         <v>0.496</v>
@@ -3719,10 +3731,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="L20" s="12">
         <v>1.4E-2</v>
@@ -3761,10 +3773,10 @@
         <v>22</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>472</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>473</v>
       </c>
       <c r="L21" s="12">
         <v>1.2999999999999999E-2</v>
@@ -3800,13 +3812,13 @@
         <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="L22" s="12">
         <v>6.4000000000000001E-2</v>
@@ -3848,7 +3860,7 @@
         <v>73</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L23" s="12">
         <v>4.5999999999999999E-2</v>
@@ -3887,10 +3899,10 @@
         <v>5</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>479</v>
       </c>
       <c r="L24" s="12">
         <v>0.02</v>
@@ -3932,7 +3944,7 @@
         <v>77</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L25" s="12">
         <v>5.8999999999999997E-2</v>
@@ -3974,7 +3986,7 @@
         <v>81</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L26" s="12">
         <v>0.13500000000000001</v>
@@ -4016,7 +4028,7 @@
         <v>83</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L27" s="12">
         <v>0.14799999999999999</v>
@@ -4055,10 +4067,10 @@
         <v>22</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="L28" s="12">
         <v>1.7000000000000001E-2</v>
@@ -4100,7 +4112,7 @@
         <v>88</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L29" s="12">
         <v>0.17</v>
@@ -4136,10 +4148,10 @@
         <v>11</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L30" s="12">
         <v>0.496</v>
@@ -4181,7 +4193,7 @@
         <v>92</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L31" s="12">
         <v>0.20300000000000001</v>
@@ -4220,7 +4232,7 @@
         <v>95</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L32" s="12">
         <v>4.3999999999999997E-2</v>
@@ -4262,7 +4274,7 @@
         <v>85</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L33" s="12">
         <v>1.2999999999999999E-2</v>
@@ -4304,7 +4316,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L34" s="12">
         <v>0.13600000000000001</v>
@@ -4343,10 +4355,10 @@
         <v>22</v>
       </c>
       <c r="J35" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="L35" s="12">
         <v>6.6000000000000003E-2</v>
@@ -4382,10 +4394,10 @@
         <v>5</v>
       </c>
       <c r="J36" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="L36" s="12">
         <v>0.161</v>
@@ -4424,10 +4436,10 @@
         <v>22</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="L37" s="12">
         <v>1.4E-2</v>
@@ -4466,10 +4478,10 @@
         <v>22</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L38" s="12">
         <v>3.1E-2</v>
@@ -4480,7 +4492,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="18">
+      <c r="A39" s="20">
         <v>38</v>
       </c>
       <c r="B39" s="7">
@@ -4496,13 +4508,13 @@
         <v>112</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>113</v>
+        <v>639</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>111</v>
+        <v>640</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="L39" s="12">
         <v>0.187</v>
@@ -4513,29 +4525,39 @@
       </c>
     </row>
     <row r="40" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
+      <c r="A40" s="18">
         <v>39</v>
       </c>
       <c r="B40" s="17">
         <v>2</v>
       </c>
       <c r="C40" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="E40" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="H40" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="E40" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>607</v>
+      <c r="I40" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="J40" s="17" t="s">
-        <v>605</v>
+        <v>641</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>612</v>
+        <v>642</v>
+      </c>
+      <c r="L40" s="17">
+        <v>0.53</v>
+      </c>
+      <c r="M40" s="17">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -4546,25 +4568,25 @@
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="J41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L41" s="12">
         <v>0.32300000000000001</v>
@@ -4582,25 +4604,25 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="I42" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L42" s="12">
         <v>0.76900000000000002</v>
@@ -4618,22 +4640,22 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="H43" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L43" s="12">
         <v>0.55000000000000004</v>
@@ -4651,22 +4673,22 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>499</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>500</v>
       </c>
       <c r="L44" s="12">
         <v>0.15</v>
@@ -4684,19 +4706,19 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="J45" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L45" s="12">
         <v>0.38</v>
@@ -4714,19 +4736,19 @@
         <v>3</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="J46" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L46" s="12">
         <v>0.249</v>
@@ -4744,25 +4766,25 @@
         <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="J47" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L47" s="12">
         <v>5.5E-2</v>
@@ -4780,25 +4802,25 @@
         <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="I48" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L48" s="12">
         <v>0.06</v>
@@ -4816,22 +4838,22 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="J49" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="L49" s="12">
         <v>1.1599999999999999</v>
@@ -4849,19 +4871,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L50" s="12">
         <v>0.188</v>
@@ -4879,19 +4901,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="J51" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L51" s="12">
         <v>1.76</v>
@@ -4909,22 +4931,22 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="I52" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L52" s="12">
         <v>0.995</v>
@@ -4942,22 +4964,22 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="K53" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L53" s="12">
         <v>1.9</v>
@@ -4975,19 +4997,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="J54" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L54" s="12">
         <v>1.5</v>
@@ -5005,22 +5027,22 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="I55" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L55" s="12">
         <v>1.236</v>
@@ -5038,22 +5060,22 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="H56" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L56" s="12">
         <v>3.5110000000000001</v>
@@ -5071,19 +5093,19 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="J57" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L57" s="12">
         <v>1.262</v>
@@ -5101,19 +5123,19 @@
         <v>2</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="J58" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L58" s="12">
         <v>1.2509999999999999</v>
@@ -5131,16 +5153,16 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="H59" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L59" s="12">
         <v>1.76</v>
@@ -5151,35 +5173,35 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="A60" s="19">
         <v>59</v>
       </c>
       <c r="B60" s="7">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F60" s="2">
         <v>0.2</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="K60" s="1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="L60" s="12">
         <v>2.13</v>
@@ -5197,28 +5219,28 @@
         <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F61" s="2">
         <v>0.2</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="K61" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L61" s="12">
         <v>0.81</v>
@@ -5229,29 +5251,29 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
+      <c r="A62" s="19">
         <v>61</v>
       </c>
       <c r="B62" s="7">
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="H62" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="K62" s="1" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="L62" s="12">
         <v>1.17</v>
@@ -5262,26 +5284,26 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="20">
+      <c r="A63" s="19">
         <v>62</v>
       </c>
       <c r="B63" s="7">
         <v>3</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="H63" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="L63" s="12">
         <v>0.96</v>
@@ -5299,25 +5321,25 @@
         <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="I64" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="K64" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L64" s="12">
         <v>5.1999999999999998E-2</v>
@@ -5335,25 +5357,25 @@
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="I65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="K65" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L65" s="12">
         <v>0.185</v>
@@ -5371,25 +5393,25 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="H66" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="I66" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="J66" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L66" s="12">
         <v>0.25600000000000001</v>
@@ -5407,22 +5429,22 @@
         <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="H67" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="I67" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="K67" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L67" s="12">
         <v>0.16500000000000001</v>
@@ -5440,25 +5462,25 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I68" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="J68" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L68" s="12">
         <v>0.246</v>
@@ -5476,19 +5498,19 @@
         <v>3</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="H69" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="K69" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="L69" s="12">
         <v>0.498</v>
@@ -5506,28 +5528,28 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D70" s="1">
         <v>33</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F70" s="2">
         <v>0.05</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="L70" s="12">
         <v>0.219</v>
@@ -5545,28 +5567,28 @@
         <v>15</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="E71" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F71" s="2">
         <v>0.01</v>
       </c>
       <c r="H71" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="K71" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L71" s="12">
         <v>1.95E-2</v>
@@ -5584,28 +5606,28 @@
         <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D72" s="1">
         <v>33.200000000000003</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F72" s="2">
         <v>0.01</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L72" s="12">
         <v>8.0000000000000002E-3</v>
@@ -5623,28 +5645,28 @@
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F73" s="2">
         <v>0.05</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L73" s="12">
         <v>1.2E-2</v>
@@ -5662,28 +5684,28 @@
         <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="E74" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F74" s="2">
         <v>0.05</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L74" s="12">
         <v>6.0000000000000001E-3</v>
@@ -5694,35 +5716,35 @@
       </c>
     </row>
     <row r="75" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+      <c r="A75" s="19">
         <v>74</v>
       </c>
       <c r="B75" s="7">
         <v>2</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D75" s="1">
         <v>330</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F75" s="2">
         <v>0.05</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L75" s="12">
         <v>4.9500000000000004E-3</v>
@@ -5740,28 +5762,28 @@
         <v>3</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="E76" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F76" s="2">
         <v>0.05</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="L76" s="12">
         <v>4.4999999999999997E-3</v>
@@ -5779,28 +5801,28 @@
         <v>9</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="E77" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F77" s="2">
         <v>0.05</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L77" s="12">
         <v>6.0000000000000001E-3</v>
@@ -5818,28 +5840,28 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="E78" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F78" s="2">
         <v>0.05</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L78" s="12">
         <v>1.2E-2</v>
@@ -5857,28 +5879,28 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D79" s="1">
         <v>22</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F79" s="2">
         <v>0.01</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L79" s="12">
         <v>1.4999999999999999E-2</v>
@@ -5896,28 +5918,28 @@
         <v>2</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F80" s="2">
         <v>0.05</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L80" s="12">
         <v>1.7000000000000001E-2</v>
@@ -5935,28 +5957,28 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F81" s="2">
         <v>0.05</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L81" s="12">
         <v>1.4E-2</v>
@@ -5974,28 +5996,28 @@
         <v>13</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F82" s="2">
         <v>0.05</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L82" s="12">
         <v>8.0000000000000002E-3</v>
@@ -6013,28 +6035,28 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D83" s="1">
         <v>100</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F83" s="2">
         <v>0.01</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L83" s="12">
         <v>0.02</v>
@@ -6052,28 +6074,28 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D84" s="1">
         <v>33</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F84" s="2">
         <v>0.05</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L84" s="12">
         <v>1.4999999999999999E-2</v>
@@ -6091,28 +6113,28 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="E85" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F85" s="2">
         <v>0.05</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="L85" s="12">
         <v>1.4E-2</v>
@@ -6130,28 +6152,28 @@
         <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="E86" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F86" s="2">
         <v>0.01</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="L86" s="12">
         <v>0.02</v>
@@ -6169,28 +6191,28 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="F87" s="2">
         <v>0.01</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L87" s="12">
         <v>2.4E-2</v>
@@ -6208,28 +6230,28 @@
         <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="E88" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F88" s="2">
         <v>0.05</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L88" s="12">
         <v>1.7000000000000001E-2</v>
@@ -6247,28 +6269,28 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F89" s="2">
         <v>0.01</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L89" s="12">
         <v>2.4E-2</v>
@@ -6286,28 +6308,28 @@
         <v>2</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F90" s="2">
         <v>0.01</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L90" s="12">
         <v>2.4E-2</v>
@@ -6325,28 +6347,28 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>285</v>
-      </c>
       <c r="E91" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F91" s="2">
         <v>0.01</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L91" s="12">
         <v>0.02</v>
@@ -6364,28 +6386,28 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="E92" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F92" s="2">
         <v>0.01</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L92" s="12">
         <v>2.4E-2</v>
@@ -6403,28 +6425,28 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="E93" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F93" s="2">
         <v>0.01</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L93" s="12">
         <v>2.4E-2</v>
@@ -6442,28 +6464,28 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E94" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F94" s="2">
         <v>0.05</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K94" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L94" s="12">
         <v>0.02</v>
@@ -6473,7 +6495,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -6481,28 +6503,28 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D95" s="1">
         <v>100</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F95" s="2">
         <v>0.05</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="L95" s="12">
         <v>1.7000000000000001E-2</v>
@@ -6520,28 +6542,28 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F96" s="2">
         <v>0.05</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J96" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="K96" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="K96" s="1" t="s">
-        <v>531</v>
       </c>
       <c r="L96" s="12">
         <v>1.2E-2</v>
@@ -6559,28 +6581,28 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="E97" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F97" s="2">
         <v>0.05</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L97" s="12">
         <v>0.02</v>
@@ -6598,28 +6620,28 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F98" s="2">
         <v>0.01</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L98" s="12">
         <v>1.7000000000000001E-2</v>
@@ -6637,28 +6659,28 @@
         <v>2</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="E99" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F99" s="2">
         <v>0.01</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K99" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L99" s="12">
         <v>1.4999999999999999E-2</v>
@@ -6676,28 +6698,28 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="E100" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F100" s="2">
         <v>0.05</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K100" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L100" s="12">
         <v>0.02</v>
@@ -6715,28 +6737,28 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F101" s="2">
         <v>0.05</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L101" s="12">
         <v>0.02</v>
@@ -6754,28 +6776,28 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F102" s="2">
         <v>0.01</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L102" s="12">
         <v>1.4999999999999999E-2</v>
@@ -6793,28 +6815,28 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="E103" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F103" s="2">
         <v>0.05</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L103" s="12">
         <v>1.2E-2</v>
@@ -6832,28 +6854,28 @@
         <v>3</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D104" s="1">
         <v>12</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F104" s="2">
         <v>0.05</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L104" s="12">
         <v>0.02</v>
@@ -6871,28 +6893,28 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F105" s="2">
         <v>0.05</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L105" s="12">
         <v>1.7000000000000001E-2</v>
@@ -6910,28 +6932,28 @@
         <v>1</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E106" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F106" s="2">
         <v>0.05</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>67</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L106" s="12">
         <v>1.7000000000000001E-2</v>
@@ -6949,28 +6971,28 @@
         <v>28</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D107" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F107" s="2">
         <v>0.05</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K107" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L107" s="12">
         <v>3.1E-2</v>
@@ -6988,28 +7010,28 @@
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F108" s="2">
         <v>0.05</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L108" s="12">
         <v>1.7000000000000001E-2</v>
@@ -7027,28 +7049,28 @@
         <v>5</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D109" s="1">
         <v>20</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F109" s="2">
         <v>0.01</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L109" s="12">
         <v>4.1000000000000002E-2</v>
@@ -7066,28 +7088,28 @@
         <v>1</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D110" s="1">
         <v>160</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F110" s="2">
         <v>0.01</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L110" s="12">
         <v>4.3999999999999997E-2</v>
@@ -7105,25 +7127,25 @@
         <v>3</v>
       </c>
       <c r="C111" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="F111" s="2">
         <v>0.01</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I111" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="J111" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="J111" s="1" t="s">
-        <v>549</v>
-      </c>
       <c r="K111" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L111" s="12">
         <v>1.2999999999999999E-2</v>
@@ -7141,25 +7163,25 @@
         <v>18</v>
       </c>
       <c r="C112" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="F112" s="2">
         <v>0.01</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="L112" s="12">
         <v>6.0000000000000001E-3</v>
@@ -7177,25 +7199,25 @@
         <v>3</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F113" s="2">
         <v>0.01</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L113" s="12">
         <v>1.4999999999999999E-2</v>
@@ -7213,25 +7235,25 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F114" s="2">
         <v>0.01</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="L114" s="12">
         <v>1.6E-2</v>
@@ -7249,25 +7271,25 @@
         <v>3</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="F115" s="2">
         <v>0.01</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L115" s="12">
         <v>1.2999999999999999E-2</v>
@@ -7285,25 +7307,25 @@
         <v>3</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="F116" s="2">
         <v>0.01</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L116" s="12">
         <v>1.2999999999999999E-2</v>
@@ -7321,25 +7343,25 @@
         <v>3</v>
       </c>
       <c r="C117" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="F117" s="2">
         <v>0.01</v>
       </c>
       <c r="H117" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="J117" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="I117" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J117" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="K117" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L117" s="12">
         <v>0.74</v>
@@ -7349,7 +7371,7 @@
         <v>2.2199999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -7357,25 +7379,25 @@
         <v>2</v>
       </c>
       <c r="C118" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="F118" s="2">
         <v>0.01</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="L118" s="12">
         <v>1.6E-2</v>
@@ -7393,28 +7415,28 @@
         <v>1</v>
       </c>
       <c r="C119" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="E119" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F119" s="2">
         <v>0.01</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K119" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L119" s="12">
         <v>2.4E-2</v>
@@ -7432,28 +7454,28 @@
         <v>1</v>
       </c>
       <c r="C120" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="E120" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F120" s="2">
         <v>0.01</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K120" s="8" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L120" s="12">
         <v>2.4E-2</v>
@@ -7471,22 +7493,22 @@
         <v>2</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D121" s="1">
         <v>22</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L121" s="12">
         <v>0.24399999999999999</v>
@@ -7496,7 +7518,7 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -7504,22 +7526,22 @@
         <v>2</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D122" s="1">
         <v>0</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="M122" s="5">
         <f t="shared" si="1"/>
@@ -7534,22 +7556,22 @@
         <v>2</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L123" s="12">
         <v>0.24399999999999999</v>
@@ -7567,22 +7589,22 @@
         <v>2</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>365</v>
-      </c>
       <c r="H124" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L124" s="12">
         <v>0.24399999999999999</v>
@@ -7600,19 +7622,19 @@
         <v>1</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="L125" s="12">
         <v>0</v>
@@ -7629,22 +7651,22 @@
         <v>2</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="H126" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J126" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="K126" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="L126" s="12">
         <v>0.497</v>
@@ -7662,19 +7684,19 @@
         <v>1</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="H127" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="H127" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="J127" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L127" s="12">
         <v>81.83</v>
@@ -7685,26 +7707,26 @@
       </c>
     </row>
     <row r="128" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A128" s="20">
+      <c r="A128" s="19">
         <v>132</v>
       </c>
       <c r="B128" s="7">
         <v>2</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="H128" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H128" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="J128" s="1" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="L128" s="12">
         <v>3.35</v>
@@ -7722,22 +7744,22 @@
         <v>1</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="H129" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H129" s="1" t="s">
+      <c r="I129" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="I129" s="1" t="s">
-        <v>379</v>
-      </c>
       <c r="J129" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L129" s="12">
         <v>0.505</v>
@@ -7755,22 +7777,22 @@
         <v>2</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="H130" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H130" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="I130" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L130" s="12">
         <v>0.26500000000000001</v>
@@ -7788,19 +7810,19 @@
         <v>1</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="H131" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="H131" s="1" t="s">
-        <v>385</v>
-      </c>
       <c r="J131" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L131" s="12">
         <v>1.06</v>
@@ -7818,19 +7840,19 @@
         <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="H132" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H132" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="J132" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L132" s="12">
         <v>2.33</v>
@@ -7848,22 +7870,22 @@
         <v>1</v>
       </c>
       <c r="C133" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D133" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="H133" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L133" s="12">
         <v>2.59</v>
@@ -7881,22 +7903,22 @@
         <v>1</v>
       </c>
       <c r="C134" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="H134" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L134" s="12">
         <v>0.28399999999999997</v>
@@ -7906,7 +7928,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>139</v>
       </c>
@@ -7914,22 +7936,22 @@
         <v>1</v>
       </c>
       <c r="C135" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="H135" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="H135" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="I135" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="L135" s="12">
         <v>4.72</v>
@@ -7947,22 +7969,22 @@
         <v>1</v>
       </c>
       <c r="C136" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="H136" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="H136" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="I136" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L136" s="12">
         <v>1.1200000000000001</v>
@@ -7980,22 +8002,22 @@
         <v>1</v>
       </c>
       <c r="C137" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="H137" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="H137" s="1" t="s">
-        <v>401</v>
-      </c>
       <c r="I137" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L137" s="12">
         <v>0.94099999999999995</v>
@@ -8005,7 +8027,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>142</v>
       </c>
@@ -8013,19 +8035,19 @@
         <v>1</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="H138" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="H138" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="J138" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="L138" s="12">
         <v>0.28399999999999997</v>
@@ -8043,22 +8065,22 @@
         <v>1</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="H139" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="H139" s="1" t="s">
-        <v>407</v>
-      </c>
       <c r="I139" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L139" s="12">
         <v>0.35</v>
@@ -8076,22 +8098,22 @@
         <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="H140" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="H140" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="I140" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L140" s="12">
         <v>3.93</v>
@@ -8109,22 +8131,22 @@
         <v>1</v>
       </c>
       <c r="C141" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="H141" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="H141" s="1" t="s">
+      <c r="I141" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="J141" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I141" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="J141" s="1" t="s">
-        <v>414</v>
-      </c>
       <c r="K141" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L141" s="12">
         <v>0.56200000000000006</v>
@@ -8142,22 +8164,22 @@
         <v>1</v>
       </c>
       <c r="C142" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="H142" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="H142" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="I142" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L142" s="12">
         <v>1.07</v>
@@ -8167,7 +8189,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>147</v>
       </c>
@@ -8175,19 +8197,19 @@
         <v>3</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="H143" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="H143" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="J143" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="L143" s="12">
         <v>5.62</v>
@@ -8205,19 +8227,19 @@
         <v>1</v>
       </c>
       <c r="C144" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>422</v>
-      </c>
       <c r="H144" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L144" s="12">
         <v>0.28399999999999997</v>
@@ -8235,19 +8257,19 @@
         <v>1</v>
       </c>
       <c r="C145" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="H145" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="H145" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="J145" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L145" s="12">
         <v>3.07</v>
@@ -8257,7 +8279,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>150</v>
       </c>
@@ -8265,22 +8287,22 @@
         <v>1</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="H146" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="H146" s="1" t="s">
-        <v>428</v>
-      </c>
       <c r="I146" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="L146" s="12">
         <v>0.28799999999999998</v>
@@ -8298,22 +8320,22 @@
         <v>1</v>
       </c>
       <c r="C147" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="H147" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="H147" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="I147" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L147" s="12">
         <v>9.8699999999999992</v>
@@ -8331,22 +8353,22 @@
         <v>1</v>
       </c>
       <c r="C148" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="H148" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="H148" s="1" t="s">
-        <v>434</v>
-      </c>
       <c r="I148" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="K148" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="J148" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="K148" s="1" t="s">
-        <v>561</v>
       </c>
       <c r="L148" s="12">
         <v>0.68500000000000005</v>
@@ -8364,22 +8386,22 @@
         <v>1</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>436</v>
-      </c>
       <c r="H149" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L149" s="12">
         <v>0.79</v>

</xml_diff>